<commit_message>
numbers ver 1.0.0 release
OK
</commit_message>
<xml_diff>
--- a/numbers/template.xlsx
+++ b/numbers/template.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{244021C7-7680-C748-A18B-1FA6C6467437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{03405397-603E-FF43-9127-5C845A5E198B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="3x3" sheetId="2" r:id="rId1"/>
-    <sheet name="3x4" sheetId="12" r:id="rId2"/>
-    <sheet name="4x4" sheetId="11" r:id="rId3"/>
-    <sheet name="5x5" sheetId="24" r:id="rId4"/>
-    <sheet name="3x3x3" sheetId="22" r:id="rId5"/>
-    <sheet name="3x3x4" sheetId="15" r:id="rId6"/>
-    <sheet name="3x3x5" sheetId="18" r:id="rId7"/>
-    <sheet name="3x3x8" sheetId="23" r:id="rId8"/>
+    <sheet name="version" sheetId="25" r:id="rId1"/>
+    <sheet name="3x3" sheetId="2" r:id="rId2"/>
+    <sheet name="3x4" sheetId="12" r:id="rId3"/>
+    <sheet name="4x4" sheetId="11" r:id="rId4"/>
+    <sheet name="5x5" sheetId="24" r:id="rId5"/>
+    <sheet name="3x3x3" sheetId="22" r:id="rId6"/>
+    <sheet name="3x3x4" sheetId="15" r:id="rId7"/>
+    <sheet name="3x3x5" sheetId="18" r:id="rId8"/>
+    <sheet name="3x3x8" sheetId="23" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3426" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3429" uniqueCount="781">
   <si>
     <t>T</t>
   </si>
@@ -2369,6 +2370,15 @@
   </si>
   <si>
     <t>AH22</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>新規作成</t>
   </si>
 </sst>
 </file>
@@ -2554,7 +2564,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2619,6 +2629,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2934,11 +2947,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE41A3B-F45E-134D-9021-37AAA8EF9585}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.15234375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>779</v>
+      </c>
+      <c r="B2" s="22">
+        <v>45286</v>
+      </c>
+      <c r="C2" t="s">
+        <v>780</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAFA817-EC99-6C46-9F70-A3B111FC0BA5}">
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4357,11 +4404,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F735F4-EEBF-2E48-8A18-F13F826D99ED}">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -6786,7 +6833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793BA828-2145-7849-A5D3-4C70578DADCC}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
@@ -10999,7 +11046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E713AC-26CA-564C-858F-FFB4808EF383}">
   <dimension ref="A1:Z119"/>
   <sheetViews>
@@ -20939,7 +20986,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22188AAF-0828-5640-A1B1-5B5F1D7DC658}">
   <dimension ref="A1:P101"/>
   <sheetViews>
@@ -25005,7 +25052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A946942D-41DB-9345-9E20-F456D170F89C}">
   <dimension ref="A1:V126"/>
   <sheetViews>
@@ -30353,7 +30400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49FF5DC-A738-9143-A7EF-1B655C169FA6}">
   <dimension ref="A1:V153"/>
   <sheetViews>
@@ -36983,7 +37030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B433D4F7-E615-6D4F-8768-8F6E818087CD}">
   <dimension ref="A1:AH230"/>
   <sheetViews>

</xml_diff>